<commit_message>
Minor update: Added clarifications on spreadsheet template
</commit_message>
<xml_diff>
--- a/public/static/waste-upload-template.xlsx
+++ b/public/static/waste-upload-template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\GreenCycle-Dashboard\public\static\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71168C6C-5F85-4A60-BC7B-27E4DC89349C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5A2AC7A-99F4-495C-85A1-3C77C81F467E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
   <si>
     <t>Population (based on Census)</t>
   </si>
@@ -167,13 +167,86 @@
   </si>
   <si>
     <t>Other (Special / Hazardous)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Please enter the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="5" tint="-0.249977111117893"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>raw waste amounts</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="5" tint="-0.249977111117893"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> below. Values must be in </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="5" tint="-0.249977111117893"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>kilograms</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="5" tint="-0.249977111117893"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Please provide population as a </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="5" tint="-0.249977111117893"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>whole number</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="5" tint="-0.249977111117893"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. Commas are considered invalid.</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -196,6 +269,21 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="5" tint="-0.249977111117893"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="5" tint="-0.249977111117893"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -357,7 +445,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -380,6 +468,8 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -601,7 +691,7 @@
   <dimension ref="B2:I42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -618,6 +708,9 @@
         <v>0</v>
       </c>
       <c r="C2" s="2"/>
+      <c r="D2" s="15" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
@@ -630,6 +723,11 @@
         <v>2</v>
       </c>
       <c r="C4" s="2"/>
+    </row>
+    <row r="6" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D6" s="14" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B7" s="7" t="s">
@@ -1093,5 +1191,6 @@
     <mergeCell ref="B28:B33"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>